<commit_message>
Scrape data project update
</commit_message>
<xml_diff>
--- a/UDACITY_Projects/Invoice Scraping Project/data_folder/JaneDoe130792.xlsx
+++ b/UDACITY_Projects/Invoice Scraping Project/data_folder/JaneDoe130792.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FLI028\Desktop\RPA_projects\UDACITY_Projects\Invoice Scraping Project\data_folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FLI028\Desktop\RPA_Udacity_projects\UDACITY_Projects\Invoice Scraping Project\data_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71639E5-3694-4C39-A3ED-AA3E6717156F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA4675-825D-480D-8E54-E820DF4200EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1330" yWindow="750" windowWidth="14400" windowHeight="7820" xr2:uid="{943E161D-9874-4E3A-94AE-8F84E050F570}"/>
+    <workbookView xWindow="1330" yWindow="750" windowWidth="14400" windowHeight="7820" xr2:uid="{7082AD52-0748-4E2D-B742-3D61B25BFFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>InvoiceNo</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Sep 01, 2020</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST 8% </t>
   </si>
 </sst>
 </file>
@@ -399,34 +393,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABC7D87-ADAA-4F2D-AA52-FE11000913B6}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBB2081-C5C0-46E4-97BC-E1923B3C564B}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>130792</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>